<commit_message>
refactor: jdbc template 적용
</commit_message>
<xml_diff>
--- a/excelfiles/test.xlsx
+++ b/excelfiles/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryu/ExcelManager/excelfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{320E0E87-7D4D-D84B-8E2D-4A9BE6629A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE958803-292D-B74C-B4F8-EDF9175EAD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16260" xr2:uid="{8F6D5AC7-EE5E-A447-BFD2-677187273057}"/>
   </bookViews>
@@ -36,9 +36,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㅇ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㅁ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㄴ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㄹ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㅎ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -403,22 +423,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB231BF-933F-4643-ADBB-79E85DD390F4}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>